<commit_message>
EPBDS-7993 Use [] to escape special symbols
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Strings_like.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Strings_like.xlsx
@@ -160,13 +160,13 @@
     <t>+##(###) ###-##-##</t>
   </si>
   <si>
-    <t>?+\@?+.?+</t>
-  </si>
-  <si>
-    <t>*\@*.*</t>
-  </si>
-  <si>
-    <t>@+\@@+.@+</t>
+    <t>@+[@]@+.@+</t>
+  </si>
+  <si>
+    <t>?+[@]?+.?+</t>
+  </si>
+  <si>
+    <t>*[@]*.*</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
   <dimension ref="B3:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -749,7 +749,7 @@
         <v>26</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -760,7 +760,7 @@
         <v>27</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -768,21 +768,21 @@
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="E24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="E25" t="b">
         <v>1</v>
@@ -790,10 +790,10 @@
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="E26" t="b">
         <v>1</v>
@@ -801,21 +801,21 @@
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C28" s="1" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="E28" t="b">
         <v>1</v>
@@ -823,10 +823,10 @@
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C29" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E29" t="b">
         <v>1</v>
@@ -834,10 +834,10 @@
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
@@ -845,10 +845,10 @@
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E31" t="b">
         <v>1</v>
@@ -856,10 +856,10 @@
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C32" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E32" t="b">
         <v>1</v>
@@ -867,10 +867,10 @@
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C33" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E33" t="b">
         <v>1</v>
@@ -878,10 +878,10 @@
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E34" t="b">
         <v>1</v>
@@ -889,10 +889,10 @@
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C35" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E35" t="b">
         <v>1</v>
@@ -900,10 +900,10 @@
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="E36" t="b">
         <v>1</v>
@@ -911,10 +911,10 @@
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C37" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="E37" t="b">
         <v>1</v>
@@ -922,10 +922,10 @@
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C38" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="E38" t="b">
         <v>1</v>
@@ -933,10 +933,10 @@
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C39" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E39" t="b">
         <v>1</v>
@@ -944,10 +944,10 @@
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C40" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E40" t="b">
         <v>1</v>
@@ -955,10 +955,10 @@
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C41" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E41" t="b">
         <v>1</v>

</xml_diff>